<commit_message>
Removed unused code from notebook
</commit_message>
<xml_diff>
--- a/Statistical_Significance_OLS.xlsx
+++ b/Statistical_Significance_OLS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\University Studies\Spring 2023\Independent Study Revival\Github\Agriculture-Data-Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65BD633E-7806-4586-9FC2-C5B755D45D62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{364F7B39-8240-41F1-BEB2-E46966EB1B54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10" yWindow="10" windowWidth="19180" windowHeight="10060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Precipitation</t>
   </si>
@@ -72,16 +72,22 @@
     <t>Statistically Significant Factor</t>
   </si>
   <si>
-    <t>1. Maize(corn) : Can be grown using less volume of water.</t>
-  </si>
-  <si>
-    <t>2. Sugarcane: Can be grown using less volume of water.</t>
-  </si>
-  <si>
-    <t>3. Sweet potatoes: Can be grown using less fertilizers.</t>
-  </si>
-  <si>
     <t>Inferences: (Based purely on statistical data and not on domain knowledge)</t>
+  </si>
+  <si>
+    <t>1. Maize(corn) : Can be grown using less volume of water, precipitation has negative impact on corn yield.</t>
+  </si>
+  <si>
+    <t>2. Rice: Gross enrolment ratio is a significant positive predictor.</t>
+  </si>
+  <si>
+    <t>3. Sugar Cane: Precipitation and water use efficiency  are major negative predictors which means sugarcane requires more water to grow.</t>
+  </si>
+  <si>
+    <t>4. Bananas: Requires high amount of government expenditure as Agriculture share of Government Expenditure is a significant positive predictor.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5. Sweet Potatoes: Precipitation has negative impact on its yield. Gross enrolment ratio is a significant positive predictor.  </t>
   </si>
 </sst>
 </file>
@@ -429,10 +435,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -630,22 +636,32 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Final commit for submission-addressing professor's remarks
</commit_message>
<xml_diff>
--- a/Statistical_Significance_OLS.xlsx
+++ b/Statistical_Significance_OLS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\University Studies\Spring 2023\Independent Study Revival\Github\Agriculture-Data-Analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{364F7B39-8240-41F1-BEB2-E46966EB1B54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{037F77DD-84BF-4A57-99C0-92A4F2C1AE2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10" yWindow="10" windowWidth="19180" windowHeight="10060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Precipitation</t>
   </si>
@@ -36,9 +36,6 @@
     <t>Avg temperature</t>
   </si>
   <si>
-    <t>Gross enrolment ratio, primary to tertiary, both sexes (%)</t>
-  </si>
-  <si>
     <t>Fertilizer Use Per Area</t>
   </si>
   <si>
@@ -78,16 +75,31 @@
     <t>1. Maize(corn) : Can be grown using less volume of water, precipitation has negative impact on corn yield.</t>
   </si>
   <si>
-    <t>2. Rice: Gross enrolment ratio is a significant positive predictor.</t>
-  </si>
-  <si>
-    <t>3. Sugar Cane: Precipitation and water use efficiency  are major negative predictors which means sugarcane requires more water to grow.</t>
-  </si>
-  <si>
-    <t>4. Bananas: Requires high amount of government expenditure as Agriculture share of Government Expenditure is a significant positive predictor.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5. Sweet Potatoes: Precipitation has negative impact on its yield. Gross enrolment ratio is a significant positive predictor.  </t>
+    <t>Credit to Agriculture</t>
+  </si>
+  <si>
+    <t>FDI inflows to Agriculture</t>
+  </si>
+  <si>
+    <t>Gini coefficient</t>
+  </si>
+  <si>
+    <t>Gross enrollment ratio, primary to tertiary, both sexes (%)</t>
+  </si>
+  <si>
+    <t>2. Rice: Fertilizer use per area  is a significant positive predictor.</t>
+  </si>
+  <si>
+    <t>3. Sugar Cane: Fertilizer use per area and water use efficiency are significant factors.</t>
+  </si>
+  <si>
+    <t>4. Bananas: Precipitation, average temperature, FDI inflows to agriculture are significant factors.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5. Sweet Potatoes: Precipitation has negative impact on its yield.  </t>
+  </si>
+  <si>
+    <t>Gross enrollment ratio, agriculture share of government expenditure, Gini coefficient are overall significant factors.</t>
   </si>
 </sst>
 </file>
@@ -435,10 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -450,11 +462,11 @@
     <col min="5" max="5" width="15.7265625" customWidth="1"/>
     <col min="6" max="6" width="15.81640625" customWidth="1"/>
     <col min="7" max="7" width="12.453125" customWidth="1"/>
-    <col min="8" max="8" width="13" customWidth="1"/>
-    <col min="9" max="9" width="15.453125" customWidth="1"/>
+    <col min="8" max="11" width="13" customWidth="1"/>
+    <col min="12" max="12" width="15.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
@@ -465,207 +477,266 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0.77900000000000003</v>
+      </c>
+      <c r="D2">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="E2">
+        <v>0.186</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0.98499999999999999</v>
+      </c>
+      <c r="I2">
+        <v>0.52800000000000002</v>
+      </c>
+      <c r="J2">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="K2">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="L2">
+        <v>0.60699999999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>8</v>
       </c>
-      <c r="B2">
-        <v>0</v>
-      </c>
-      <c r="C2">
-        <v>0.499</v>
-      </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
+      <c r="B3">
+        <v>0.22</v>
+      </c>
+      <c r="C3">
+        <v>0.1</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3">
+        <v>0.61199999999999999</v>
+      </c>
+      <c r="H3">
+        <v>0.96099999999999997</v>
+      </c>
+      <c r="I3">
+        <v>0.85499999999999998</v>
+      </c>
+      <c r="J3">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0.64500000000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4">
+        <v>0.12</v>
+      </c>
+      <c r="C4">
+        <v>1.4E-2</v>
+      </c>
+      <c r="D4">
+        <v>9.9000000000000005E-2</v>
+      </c>
+      <c r="E4">
+        <v>2.4E-2</v>
+      </c>
+      <c r="F4">
+        <v>1E-3</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0.58499999999999996</v>
+      </c>
+      <c r="I4">
+        <v>0.30299999999999999</v>
+      </c>
+      <c r="J4">
+        <v>0.19400000000000001</v>
+      </c>
+      <c r="K4">
         <v>2E-3</v>
       </c>
-      <c r="G2">
-        <v>1.0999999999999999E-2</v>
-      </c>
-      <c r="H2">
-        <v>0</v>
-      </c>
-      <c r="I2">
-        <v>0.55428943200620295</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>0.115</v>
-      </c>
-      <c r="D3">
-        <v>0</v>
-      </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>0.29499999999999998</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>0.46076762284622702</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="L4">
+        <v>0.46500000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>10</v>
       </c>
-      <c r="B4">
-        <v>2.5999999999999999E-2</v>
-      </c>
-      <c r="C4">
-        <v>0.61699999999999999</v>
-      </c>
-      <c r="D4">
-        <v>3.5999999999999997E-2</v>
-      </c>
-      <c r="E4">
-        <v>8.0000000000000002E-3</v>
-      </c>
-      <c r="F4">
-        <v>0.13700000000000001</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>7.2533654569685593E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>2E-3</v>
+      </c>
+      <c r="D5">
+        <v>2E-3</v>
+      </c>
+      <c r="E5">
+        <v>0.93600000000000005</v>
+      </c>
+      <c r="F5">
+        <v>0.255</v>
+      </c>
+      <c r="G5">
+        <v>0.63300000000000001</v>
+      </c>
+      <c r="H5">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="I5">
+        <v>0.39500000000000002</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0.495</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
         <v>11</v>
       </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>0</v>
-      </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
-      <c r="E5">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>0.77200000000000002</v>
-      </c>
-      <c r="H5">
-        <v>0</v>
-      </c>
-      <c r="I5">
-        <v>0.34786921414151001</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>12</v>
-      </c>
       <c r="B6">
         <v>0</v>
       </c>
       <c r="C6">
-        <v>0.39600000000000002</v>
+        <v>1E-3</v>
       </c>
       <c r="D6">
         <v>0</v>
       </c>
       <c r="E6">
-        <v>0.94099999999999995</v>
+        <v>0</v>
       </c>
       <c r="F6">
-        <v>0.75700000000000001</v>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="G6">
-        <v>0.185</v>
+        <v>0</v>
       </c>
       <c r="H6">
-        <v>0</v>
+        <v>0.98299999999999998</v>
       </c>
       <c r="I6">
-        <v>0.22482517449723899</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <v>1E-3</v>
+      </c>
+      <c r="L6">
+        <v>0.73699999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="29" x14ac:dyDescent="0.35">
       <c r="B9" s="4"/>
       <c r="C9" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A11" s="2" t="s">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>20</v>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>24</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:I6">
+  <conditionalFormatting sqref="B2:L6">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="between">
       <formula>0</formula>
       <formula>0.05</formula>

</xml_diff>